<commit_message>
Updated the teaching information
</commit_message>
<xml_diff>
--- a/teaching/teaching.xlsx
+++ b/teaching/teaching.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="41">
   <si>
     <t>Year</t>
   </si>
@@ -115,6 +115,33 @@
   </si>
   <si>
     <t>Programming for engineers I</t>
+  </si>
+  <si>
+    <t>Computer Science I </t>
+  </si>
+  <si>
+    <t>West Chester University</t>
+  </si>
+  <si>
+    <t>CSC141</t>
+  </si>
+  <si>
+    <t>CSC231</t>
+  </si>
+  <si>
+    <t>Computer Systems</t>
+  </si>
+  <si>
+    <t>Computer Science III</t>
+  </si>
+  <si>
+    <t>CSC240</t>
+  </si>
+  <si>
+    <t>CSC490</t>
+  </si>
+  <si>
+    <t>Independent Project in Computer Science</t>
   </si>
 </sst>
 </file>
@@ -432,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,6 +914,91 @@
         <v>31</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2021</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2021</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2021</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2021</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2021</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>